<commit_message>
Slight update on valves
</commit_message>
<xml_diff>
--- a/K1/FinalCodeV1/Final_OutputV3.xlsx
+++ b/K1/FinalCodeV1/Final_OutputV3.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc Thomson\Documents\School Docs\College\Senior Year\Second Semester\Design\DesignCode\K1\FinalCodeV1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EEAFFD-B707-436D-B2B8-D21341DBEADD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B605C52-BEDD-466C-97BC-C32778253A01}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="5" xr2:uid="{246BD7EC-0C2E-4070-B711-658E9931285D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="4" xr2:uid="{246BD7EC-0C2E-4070-B711-658E9931285D}"/>
   </bookViews>
   <sheets>
     <sheet name="Seed Train" sheetId="1" r:id="rId1"/>
     <sheet name="Reactors" sheetId="2" r:id="rId2"/>
     <sheet name="Feed &amp; Media Composition" sheetId="3" r:id="rId3"/>
     <sheet name="PID &amp; Gas Output" sheetId="4" r:id="rId4"/>
-    <sheet name="Reactor Heating" sheetId="6" r:id="rId5"/>
-    <sheet name="Reactor Dim" sheetId="5" r:id="rId6"/>
+    <sheet name="Reactor Dim" sheetId="5" r:id="rId5"/>
+    <sheet name="Reactor Heating" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="128">
   <si>
     <t>Vessel</t>
   </si>
@@ -176,12 +176,6 @@
     <t>BatchReactor</t>
   </si>
   <si>
-    <t>MinBubble</t>
-  </si>
-  <si>
-    <t>MaxBubble</t>
-  </si>
-  <si>
     <t>ImpellerRatio</t>
   </si>
   <si>
@@ -218,15 +212,6 @@
     <t>Kd Flow</t>
   </si>
   <si>
-    <t>Flow_O2</t>
-  </si>
-  <si>
-    <t>Flow_CO2</t>
-  </si>
-  <si>
-    <t>Flow_air</t>
-  </si>
-  <si>
     <t>Max N (rpm)</t>
   </si>
   <si>
@@ -272,15 +257,6 @@
     <t>N Impeller</t>
   </si>
   <si>
-    <t>max flow CO2</t>
-  </si>
-  <si>
-    <t>max flow air</t>
-  </si>
-  <si>
-    <t>max Flow O2</t>
-  </si>
-  <si>
     <t>ST Perf 20</t>
   </si>
   <si>
@@ -359,18 +335,6 @@
     <t>Total Duty (J)</t>
   </si>
   <si>
-    <t>min Flow O2</t>
-  </si>
-  <si>
-    <t>min flow CO2</t>
-  </si>
-  <si>
-    <t>min flow air</t>
-  </si>
-  <si>
-    <t>average flow air</t>
-  </si>
-  <si>
     <t>esimate density (g/L)</t>
   </si>
   <si>
@@ -392,19 +356,64 @@
     <t>total drop</t>
   </si>
   <si>
-    <t>av flow (SCFS)</t>
-  </si>
-  <si>
     <t>Pre Pressure</t>
   </si>
   <si>
     <t>post pressure</t>
   </si>
   <si>
-    <t>xT</t>
-  </si>
-  <si>
     <t>standard density air</t>
+  </si>
+  <si>
+    <t>Max Cv</t>
+  </si>
+  <si>
+    <t>Min Cv</t>
+  </si>
+  <si>
+    <t>CV ratio</t>
+  </si>
+  <si>
+    <t>Valve</t>
+  </si>
+  <si>
+    <t>av flow (SCFH)</t>
+  </si>
+  <si>
+    <t>min Flow O2 (m^3/s)</t>
+  </si>
+  <si>
+    <t>min flow CO2 (m^3/s)</t>
+  </si>
+  <si>
+    <t>min flow air (m^3/s)</t>
+  </si>
+  <si>
+    <t>max Flow O2 (m^3/s)</t>
+  </si>
+  <si>
+    <t>max flow CO2 (m^3/s)</t>
+  </si>
+  <si>
+    <t>max flow air (m^3/s)</t>
+  </si>
+  <si>
+    <t>MinBubble (m)</t>
+  </si>
+  <si>
+    <t>MaxBubble (m)</t>
+  </si>
+  <si>
+    <t>Total Flow O2 (m^3)</t>
+  </si>
+  <si>
+    <t>Total Flow CO2  (m^3)</t>
+  </si>
+  <si>
+    <t>Total Flow air (m^3)</t>
+  </si>
+  <si>
+    <t>average flow air (m^3/s)</t>
   </si>
 </sst>
 </file>
@@ -616,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -701,6 +710,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1052,7 +1064,7 @@
         <v>0.59709999999999996</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,7 +1078,7 @@
         <v>0.43630000000000002</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1080,7 +1092,7 @@
         <v>0.4229</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1094,7 +1106,7 @@
         <v>0.42280000000000001</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1108,7 +1120,7 @@
         <v>0.4163</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1122,12 +1134,12 @@
         <v>0.41599999999999998</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B8">
         <v>2.4550000000000001</v>
@@ -1136,7 +1148,7 @@
         <v>0.44030000000000002</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,7 +1162,7 @@
         <v>0.41470000000000001</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,12 +1176,12 @@
         <v>0.44019999999999998</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B11">
         <v>2.4550000000000001</v>
@@ -1310,10 +1322,10 @@
         <v>41</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1537,37 +1549,37 @@
   <dimension ref="A1:AB35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1634,93 +1646,93 @@
       <c r="AB2" s="56"/>
     </row>
     <row r="3" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="46" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="H3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="K3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="L3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="N3" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="O3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="Q3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="R3" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y3" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA3" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="Q3" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="R3" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="V3" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="X3" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y3" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z3" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA3" s="10" t="s">
-        <v>65</v>
-      </c>
       <c r="AB3" s="11" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="47" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="13">
@@ -1741,7 +1753,7 @@
       <c r="G4" s="14">
         <v>0.39</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <v>2</v>
       </c>
       <c r="I4" s="15">
@@ -1806,7 +1818,7 @@
       </c>
     </row>
     <row r="5" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="47" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="13">
@@ -1827,7 +1839,7 @@
       <c r="G5" s="14">
         <v>0.35</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <v>1</v>
       </c>
       <c r="I5" s="15">
@@ -1892,8 +1904,8 @@
       </c>
     </row>
     <row r="6" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
-        <v>83</v>
+      <c r="A6" s="47" t="s">
+        <v>75</v>
       </c>
       <c r="B6" s="23">
         <v>0</v>
@@ -1913,7 +1925,7 @@
       <c r="G6" s="23">
         <v>0.45</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="13">
         <v>1</v>
       </c>
       <c r="I6" s="24">
@@ -1978,8 +1990,8 @@
       </c>
     </row>
     <row r="7" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>84</v>
+      <c r="A7" s="47" t="s">
+        <v>76</v>
       </c>
       <c r="B7" s="23">
         <v>0</v>
@@ -1999,7 +2011,7 @@
       <c r="G7" s="23">
         <v>0.45</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="13">
         <v>1</v>
       </c>
       <c r="I7" s="24">
@@ -2064,8 +2076,8 @@
       </c>
     </row>
     <row r="8" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>85</v>
+      <c r="A8" s="47" t="s">
+        <v>77</v>
       </c>
       <c r="B8" s="23">
         <v>0</v>
@@ -2085,7 +2097,7 @@
       <c r="G8" s="23">
         <v>0.7</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="13">
         <v>2</v>
       </c>
       <c r="I8" s="24">
@@ -2150,8 +2162,8 @@
       </c>
     </row>
     <row r="9" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
-        <v>86</v>
+      <c r="A9" s="47" t="s">
+        <v>78</v>
       </c>
       <c r="B9" s="57">
         <v>0</v>
@@ -2171,7 +2183,7 @@
       <c r="G9" s="14">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <v>2</v>
       </c>
       <c r="I9" s="15">
@@ -2236,8 +2248,8 @@
       </c>
     </row>
     <row r="10" spans="1:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>87</v>
+      <c r="A10" s="48" t="s">
+        <v>79</v>
       </c>
       <c r="B10" s="18">
         <v>0</v>
@@ -2257,7 +2269,7 @@
       <c r="G10" s="19">
         <v>0.35</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="18">
         <v>2</v>
       </c>
       <c r="I10" s="21">
@@ -2659,11 +2671,758 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AC2659-451F-4A9A-A90E-79F819C9DD82}">
+  <dimension ref="A1:X17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R1" t="s">
+        <v>108</v>
+      </c>
+      <c r="S1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U1" t="s">
+        <v>112</v>
+      </c>
+      <c r="V1" t="s">
+        <v>111</v>
+      </c>
+      <c r="W1" t="s">
+        <v>113</v>
+      </c>
+      <c r="X1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="31">
+        <v>2000000</v>
+      </c>
+      <c r="C2" s="32">
+        <f>(B2*4/(3*PI()))^(1/3)/100</f>
+        <v>0.94683205640999235</v>
+      </c>
+      <c r="D2" s="32">
+        <f>C2*3</f>
+        <v>2.8404961692299771</v>
+      </c>
+      <c r="E2" s="33">
+        <f>D2*9.8</f>
+        <v>27.836862458453776</v>
+      </c>
+      <c r="F2" s="31">
+        <f>'PID &amp; Gas Output'!W4</f>
+        <v>2.1061736989799401E-3</v>
+      </c>
+      <c r="G2" s="31">
+        <f>'PID &amp; Gas Output'!T4/10/24/3600</f>
+        <v>4.0133712131912962E-3</v>
+      </c>
+      <c r="H2" s="31">
+        <f>'PID &amp; Gas Output'!Z4</f>
+        <v>5.3139903719532904E-3</v>
+      </c>
+      <c r="J2">
+        <f>29*(100000+E2*1000)/(8.314*298)/1000</f>
+        <v>1.4963314936135699</v>
+      </c>
+      <c r="K2">
+        <f>29*(100000)/(8.314*288)/1000</f>
+        <v>1.2111431855237487</v>
+      </c>
+      <c r="L2">
+        <f>J2/K2</f>
+        <v>1.2354703485917677</v>
+      </c>
+      <c r="M2" s="31">
+        <f>G2*127133</f>
+        <v>510.23192244664904</v>
+      </c>
+      <c r="N2">
+        <f>E2*0.145</f>
+        <v>4.0363450564757972</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>P2+O2</f>
+        <v>5</v>
+      </c>
+      <c r="R2">
+        <f>Q2+14.7+N2-O2/2</f>
+        <v>21.236345056475798</v>
+      </c>
+      <c r="S2">
+        <f>R2-O2</f>
+        <v>16.236345056475798</v>
+      </c>
+      <c r="T2">
+        <f>M2/963*SQRT(1*537/(R2^2-S2^2))</f>
+        <v>0.89698678406218579</v>
+      </c>
+      <c r="U2">
+        <f>F2/963*SQRT(1*537/(R2^2-S2^2))*127133</f>
+        <v>0.47072893898148516</v>
+      </c>
+      <c r="V2">
+        <f>H2/963*SQRT(1*537/(R2^2-S2^2))*127133</f>
+        <v>1.1876746209293656</v>
+      </c>
+      <c r="W2">
+        <f>V2/U2</f>
+        <v>2.5230541880410704</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="31">
+        <v>500000</v>
+      </c>
+      <c r="C3" s="32">
+        <f>(B3*4/(1.5*PI()))^(1/3)/100</f>
+        <v>0.75150110119121716</v>
+      </c>
+      <c r="D3" s="32">
+        <f>C3*1.5</f>
+        <v>1.1272516517868256</v>
+      </c>
+      <c r="E3" s="33">
+        <f>D3*9.8</f>
+        <v>11.047066187510891</v>
+      </c>
+      <c r="F3" s="31">
+        <f>'PID &amp; Gas Output'!W5</f>
+        <v>6.8620111084161499E-5</v>
+      </c>
+      <c r="G3" s="31">
+        <f>'PID &amp; Gas Output'!T5/30/24/3600</f>
+        <v>3.2583983165975121E-3</v>
+      </c>
+      <c r="H3" s="31">
+        <f>'PID &amp; Gas Output'!Z5</f>
+        <v>3.6299908924129301E-3</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J8" si="0">29*(100000+E3*1000+E704)/(8.314*298)/1000</f>
+        <v>1.2998067944898537</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K8" si="1">29*(100000)/(8.314*288)/1000</f>
+        <v>1.2111431855237487</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L8" si="2">J3/K3</f>
+        <v>1.073206545704803</v>
+      </c>
+      <c r="M3" s="31">
+        <f t="shared" ref="M3:M8" si="3">G3*127133</f>
+        <v>414.24995318399152</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N8" si="4">E3*0.145</f>
+        <v>1.6018245971890792</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q8" si="5">P3+O3</f>
+        <v>5</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R8" si="6">Q3+14.7+N3-O3/2</f>
+        <v>18.801824597189079</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S8" si="7">R3-O3</f>
+        <v>13.801824597189079</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T8" si="8">M3/963*SQRT(1*537/(R3^2-S3^2))</f>
+        <v>0.78073781653662033</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U8" si="9">F3/963*SQRT(1*537/(R3^2-S3^2))*127133</f>
+        <v>1.6441917314238001E-2</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V8" si="10">H3/963*SQRT(1*537/(R3^2-S3^2))*127133</f>
+        <v>0.86977431486942502</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W8" si="11">V3/U3</f>
+        <v>52.899810785220133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="31">
+        <v>20000</v>
+      </c>
+      <c r="C4" s="32">
+        <f>C5</f>
+        <v>0.43948051003392441</v>
+      </c>
+      <c r="D4" s="32">
+        <f>B4/1000000/(C4^2*PI()/4)</f>
+        <v>0.13184415301017743</v>
+      </c>
+      <c r="E4" s="33">
+        <f>D4*9.8</f>
+        <v>1.2920726994997389</v>
+      </c>
+      <c r="F4" s="31">
+        <f>'PID &amp; Gas Output'!W6</f>
+        <v>1.43282608221107E-4</v>
+      </c>
+      <c r="G4" s="31">
+        <f>'PID &amp; Gas Output'!T6/'Seed Train'!B11/24/3600</f>
+        <v>3.3716673387102939E-4</v>
+      </c>
+      <c r="H4" s="31">
+        <f>'PID &amp; Gas Output'!Z6</f>
+        <v>9.6507230400850303E-4</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>1.1856245179899887</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>1.2111431855237487</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>0.97893009857234625</v>
+      </c>
+      <c r="M4" s="31">
+        <f t="shared" si="3"/>
+        <v>42.865018377225582</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="4"/>
+        <v>0.18735054142746213</v>
+      </c>
+      <c r="O4">
+        <f>O5+N5-N4</f>
+        <v>5.7494021657098475</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="5"/>
+        <v>5.7494021657098475</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="6"/>
+        <v>17.762051624282389</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="7"/>
+        <v>12.012649458572541</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="8"/>
+        <v>7.8836769668161513E-2</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="9"/>
+        <v>3.3502528117443753E-2</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="10"/>
+        <v>0.22565447685400389</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="11"/>
+        <v>6.7354462344742405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="31">
+        <v>100000</v>
+      </c>
+      <c r="C5" s="32">
+        <f>(B5*4/(1.5*PI()))^(1/3)/100</f>
+        <v>0.43948051003392441</v>
+      </c>
+      <c r="D5" s="32">
+        <f>C5*1.5</f>
+        <v>0.65922076505088656</v>
+      </c>
+      <c r="E5" s="33">
+        <f>D5*9.8</f>
+        <v>6.4603634974986885</v>
+      </c>
+      <c r="F5" s="31">
+        <f>'PID &amp; Gas Output'!W7</f>
+        <v>2.8072312163671299E-4</v>
+      </c>
+      <c r="G5" s="31">
+        <f>'PID &amp; Gas Output'!T7/'Seed Train'!B12/24/3600</f>
+        <v>4.4621826658897953E-4</v>
+      </c>
+      <c r="H5" s="31">
+        <f>'PID &amp; Gas Output'!Z7</f>
+        <v>9.7531859873896301E-4</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>1.2461194029588087</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>1.2111431855237487</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>1.0288786807811952</v>
+      </c>
+      <c r="M5" s="31">
+        <f t="shared" si="3"/>
+        <v>56.729066886256732</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="4"/>
+        <v>0.93675270713730974</v>
+      </c>
+      <c r="O5">
+        <v>5</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="6"/>
+        <v>18.136752707137308</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="7"/>
+        <v>13.136752707137308</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="8"/>
+        <v>0.10916746154899989</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="9"/>
+        <v>6.8679014020328236E-2</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="10"/>
+        <v>0.23861205064456636</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="11"/>
+        <v>3.47430804079307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="31">
+        <v>20000</v>
+      </c>
+      <c r="C6" s="32">
+        <f>(B6*4/(3*PI()))^(1/3)/100</f>
+        <v>0.20398878279639124</v>
+      </c>
+      <c r="D6" s="32">
+        <f>C6*3</f>
+        <v>0.61196634838917374</v>
+      </c>
+      <c r="E6" s="33">
+        <f>D6*9.8</f>
+        <v>5.9972702142139029</v>
+      </c>
+      <c r="F6" s="31">
+        <f>'PID &amp; Gas Output'!W8</f>
+        <v>3.6123153872598101E-6</v>
+      </c>
+      <c r="G6" s="31">
+        <f>'PID &amp; Gas Output'!T8/'Seed Train'!B8/24/3600</f>
+        <v>2.6205615232805545E-5</v>
+      </c>
+      <c r="H6" s="31">
+        <f>'PID &amp; Gas Output'!Z8</f>
+        <v>1.1611381670112299E-4</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>1.2406988923882749</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>1.2111431855237487</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>1.0244031483789797</v>
+      </c>
+      <c r="M6" s="31">
+        <f>G6*127133</f>
+        <v>3.3315984813922674</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>0.86960418106101589</v>
+      </c>
+      <c r="O6">
+        <f>O7+N7-N6</f>
+        <v>2.5108064107511856</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f>P6+O6+N6</f>
+        <v>3.3804105918122014</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="6"/>
+        <v>17.694611567497624</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="7"/>
+        <v>15.183805156746438</v>
+      </c>
+      <c r="T6">
+        <f>M6/963*SQRT(1*537/(R6^2-S6^2))</f>
+        <v>8.8237145256830785E-3</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="9"/>
+        <v>1.2163057219130389E-3</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="10"/>
+        <v>3.9096779905995492E-2</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="11"/>
+        <v>32.143875673381693</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="31">
+        <v>80000</v>
+      </c>
+      <c r="C7" s="32">
+        <f>(B7*4/(3*PI()))^(1/3)/100</f>
+        <v>0.32381200840070401</v>
+      </c>
+      <c r="D7" s="32">
+        <f>C7*3</f>
+        <v>0.97143602520211203</v>
+      </c>
+      <c r="E7" s="33">
+        <f>D7*9.8</f>
+        <v>9.5200730469806985</v>
+      </c>
+      <c r="F7" s="31">
+        <f>'PID &amp; Gas Output'!W9</f>
+        <v>2.7738531734872098E-4</v>
+      </c>
+      <c r="G7" s="31">
+        <f>'PID &amp; Gas Output'!T9/'Seed Train'!B9/24/3600</f>
+        <v>3.1820393691348704E-4</v>
+      </c>
+      <c r="H7" s="31">
+        <f>'PID &amp; Gas Output'!Z9</f>
+        <v>4.4930211738727498E-4</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>1.2819333276136637</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>1.2111431855237487</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>1.058449028105048</v>
+      </c>
+      <c r="M7" s="31">
+        <f t="shared" si="3"/>
+        <v>40.454221111622346</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>1.3804105918122012</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="6"/>
+        <v>17.0804105918122</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="7"/>
+        <v>15.0804105918122</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="8"/>
+        <v>0.12137972161167841</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="9"/>
+        <v>0.10580935272371787</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="10"/>
+        <v>0.17138746445752598</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="11"/>
+        <v>1.6197761355278411</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="31">
+        <v>400000</v>
+      </c>
+      <c r="C8" s="32">
+        <f>(B8*4/(3*PI()))^(1/3)/100</f>
+        <v>0.55371074561027633</v>
+      </c>
+      <c r="D8" s="32">
+        <f>C8*3</f>
+        <v>1.661132236830829</v>
+      </c>
+      <c r="E8" s="33">
+        <f>D8*9.8</f>
+        <v>16.279095920942126</v>
+      </c>
+      <c r="F8" s="31">
+        <f>'PID &amp; Gas Output'!W10</f>
+        <v>1.4599157214174199E-3</v>
+      </c>
+      <c r="G8" s="31">
+        <f>'PID &amp; Gas Output'!T10/'Seed Train'!B10/24/3600</f>
+        <v>1.5291703869733961E-3</v>
+      </c>
+      <c r="H8" s="31">
+        <f>'PID &amp; Gas Output'!Z10</f>
+        <v>1.829851947594E-3</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>1.3610477442057471</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>1.2111431855237487</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>1.1237711283634673</v>
+      </c>
+      <c r="M8" s="31">
+        <f t="shared" si="3"/>
+        <v>194.40801880708875</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>2.3604689085366082</v>
+      </c>
+      <c r="O8">
+        <f>O7+N7-N8</f>
+        <v>1.0199416832755932</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="5"/>
+        <v>1.0199416832755932</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="6"/>
+        <v>17.570439750174405</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="7"/>
+        <v>16.550498066898811</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="8"/>
+        <v>0.79300674270119698</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="9"/>
+        <v>0.75709222511882046</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="10"/>
+        <v>0.94893606686892029</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="11"/>
+        <v>1.2533956041088539</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43169691-B23A-4265-B676-8F187760D4B1}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2697,31 +3456,31 @@
         <v>17</v>
       </c>
       <c r="B3" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="41" t="s">
         <v>100</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="H3" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="I3" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="J3" s="41" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2790,7 +3549,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B6" s="23">
         <v>37.200000000000003</v>
@@ -2816,7 +3575,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B7" s="23">
         <v>37</v>
@@ -2842,7 +3601,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B8" s="23">
         <v>37</v>
@@ -2868,7 +3627,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B9" s="23">
         <v>37</v>
@@ -2894,7 +3653,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B10" s="1">
         <v>37</v>
@@ -2924,668 +3683,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AC2659-451F-4A9A-A90E-79F819C9DD82}">
-  <dimension ref="A1:T17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K1" t="s">
-        <v>124</v>
-      </c>
-      <c r="L1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M1" t="s">
-        <v>120</v>
-      </c>
-      <c r="N1" t="s">
-        <v>116</v>
-      </c>
-      <c r="O1" t="s">
-        <v>117</v>
-      </c>
-      <c r="P1" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>119</v>
-      </c>
-      <c r="R1" t="s">
-        <v>121</v>
-      </c>
-      <c r="S1" t="s">
-        <v>122</v>
-      </c>
-      <c r="T1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="31">
-        <v>2000000</v>
-      </c>
-      <c r="C2" s="32">
-        <f>(B2*4/(3*PI()))^(1/3)/100</f>
-        <v>0.94683205640999235</v>
-      </c>
-      <c r="D2" s="32">
-        <f>C2*3</f>
-        <v>2.8404961692299771</v>
-      </c>
-      <c r="E2" s="33">
-        <f>D2*9.8</f>
-        <v>27.836862458453776</v>
-      </c>
-      <c r="F2" s="31">
-        <f>'PID &amp; Gas Output'!W4</f>
-        <v>2.1061736989799401E-3</v>
-      </c>
-      <c r="G2" s="31">
-        <f>'PID &amp; Gas Output'!T4/10/24/3600</f>
-        <v>4.0133712131912962E-3</v>
-      </c>
-      <c r="H2" s="31">
-        <f>'PID &amp; Gas Output'!Z4</f>
-        <v>5.3139903719532904E-3</v>
-      </c>
-      <c r="J2">
-        <f>29*(100000+E2*1000)/(8.314*298)/1000</f>
-        <v>1.4963314936135699</v>
-      </c>
-      <c r="K2">
-        <f>29*(100000)/(8.314*288)/1000</f>
-        <v>1.2111431855237487</v>
-      </c>
-      <c r="L2">
-        <f>J2/K2</f>
-        <v>1.2354703485917677</v>
-      </c>
-      <c r="M2" s="31">
-        <f>G2*127133</f>
-        <v>510.23192244664904</v>
-      </c>
-      <c r="N2">
-        <f>E2*0.145</f>
-        <v>4.0363450564757972</v>
-      </c>
-      <c r="O2">
-        <f>R11</f>
-        <v>5</v>
-      </c>
-      <c r="P2">
-        <v>10</v>
-      </c>
-      <c r="Q2">
-        <f>P2+O2</f>
-        <v>15</v>
-      </c>
-      <c r="R2">
-        <f>Q2+14.7+N2-O2/2</f>
-        <v>31.236345056475798</v>
-      </c>
-      <c r="S2">
-        <f>R2-O2</f>
-        <v>26.236345056475798</v>
-      </c>
-      <c r="T2">
-        <f>M2/963*SQRT(1*537/(R2^2-S2^2))</f>
-        <v>0.72429038067673757</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="31">
-        <v>500000</v>
-      </c>
-      <c r="C3" s="32">
-        <f>(B3*4/(1.5*PI()))^(1/3)/100</f>
-        <v>0.75150110119121716</v>
-      </c>
-      <c r="D3" s="32">
-        <f>C3*1.5</f>
-        <v>1.1272516517868256</v>
-      </c>
-      <c r="E3" s="33">
-        <f>D3*9.8</f>
-        <v>11.047066187510891</v>
-      </c>
-      <c r="F3" s="31">
-        <f>'PID &amp; Gas Output'!W5</f>
-        <v>6.8620111084161499E-5</v>
-      </c>
-      <c r="G3" s="31">
-        <f>'PID &amp; Gas Output'!T5/30/24/3600</f>
-        <v>3.2583983165975121E-3</v>
-      </c>
-      <c r="H3" s="31">
-        <f>'PID &amp; Gas Output'!Z5</f>
-        <v>3.6299908924129301E-3</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J8" si="0">29*(100000+E3*1000+E704)/(8.314*298)/1000</f>
-        <v>1.2998067944898537</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K8" si="1">29*(100000)/(8.314*288)/1000</f>
-        <v>1.2111431855237487</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L8" si="2">J3/K3</f>
-        <v>1.073206545704803</v>
-      </c>
-      <c r="M3" s="31">
-        <f t="shared" ref="M3:M8" si="3">G3*127133</f>
-        <v>414.24995318399152</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N8" si="4">E3*0.145</f>
-        <v>1.6018245971890792</v>
-      </c>
-      <c r="O3">
-        <f>R11</f>
-        <v>5</v>
-      </c>
-      <c r="P3">
-        <v>10</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q8" si="5">P3+O3</f>
-        <v>15</v>
-      </c>
-      <c r="R3">
-        <f t="shared" ref="R3:R8" si="6">Q3+14.7+N3-O3/2</f>
-        <v>28.801824597189079</v>
-      </c>
-      <c r="S3">
-        <f t="shared" ref="S3:S8" si="7">R3-O3</f>
-        <v>23.801824597189079</v>
-      </c>
-      <c r="T3">
-        <f t="shared" ref="T3:T8" si="8">M3/963*SQRT(1*537/(R3^2-S3^2))</f>
-        <v>0.61465353705828785</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="31">
-        <v>20000</v>
-      </c>
-      <c r="C4" s="32">
-        <f>C5</f>
-        <v>0.43948051003392441</v>
-      </c>
-      <c r="D4" s="32">
-        <f>B4/1000000/(C4^2*PI()/4)</f>
-        <v>0.13184415301017743</v>
-      </c>
-      <c r="E4" s="33">
-        <f>D4*9.8</f>
-        <v>1.2920726994997389</v>
-      </c>
-      <c r="F4" s="31">
-        <f>'PID &amp; Gas Output'!W6</f>
-        <v>1.43282608221107E-4</v>
-      </c>
-      <c r="G4" s="31">
-        <f>'PID &amp; Gas Output'!T6/'Seed Train'!B11/24/3600</f>
-        <v>3.3716673387102939E-4</v>
-      </c>
-      <c r="H4" s="31">
-        <f>'PID &amp; Gas Output'!Z6</f>
-        <v>9.6507230400850303E-4</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>1.1856245179899887</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="1"/>
-        <v>1.2111431855237487</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="2"/>
-        <v>0.97893009857234625</v>
-      </c>
-      <c r="M4" s="31">
-        <f t="shared" si="3"/>
-        <v>42.865018377225582</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="4"/>
-        <v>0.18735054142746213</v>
-      </c>
-      <c r="O4">
-        <f>O5+N5-N4</f>
-        <v>5.7494021657098475</v>
-      </c>
-      <c r="P4">
-        <v>10</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="5"/>
-        <v>15.749402165709848</v>
-      </c>
-      <c r="R4">
-        <f t="shared" si="6"/>
-        <v>27.762051624282389</v>
-      </c>
-      <c r="S4">
-        <f t="shared" si="7"/>
-        <v>22.01264945857254</v>
-      </c>
-      <c r="T4">
-        <f t="shared" si="8"/>
-        <v>6.0974492677692234E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="31">
-        <v>100000</v>
-      </c>
-      <c r="C5" s="32">
-        <f>(B5*4/(1.5*PI()))^(1/3)/100</f>
-        <v>0.43948051003392441</v>
-      </c>
-      <c r="D5" s="32">
-        <f>C5*1.5</f>
-        <v>0.65922076505088656</v>
-      </c>
-      <c r="E5" s="33">
-        <f>D5*9.8</f>
-        <v>6.4603634974986885</v>
-      </c>
-      <c r="F5" s="31">
-        <f>'PID &amp; Gas Output'!W7</f>
-        <v>2.8072312163671299E-4</v>
-      </c>
-      <c r="G5" s="31">
-        <f>'PID &amp; Gas Output'!T7/'Seed Train'!B12/24/3600</f>
-        <v>4.4621826658897953E-4</v>
-      </c>
-      <c r="H5" s="31">
-        <f>'PID &amp; Gas Output'!Z7</f>
-        <v>9.7531859873896301E-4</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>1.2461194029588087</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>1.2111431855237487</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="2"/>
-        <v>1.0288786807811952</v>
-      </c>
-      <c r="M5" s="31">
-        <f t="shared" si="3"/>
-        <v>56.729066886256732</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="4"/>
-        <v>0.93675270713730974</v>
-      </c>
-      <c r="O5">
-        <f>R11</f>
-        <v>5</v>
-      </c>
-      <c r="P5">
-        <v>10</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="R5">
-        <f t="shared" si="6"/>
-        <v>28.136752707137308</v>
-      </c>
-      <c r="S5">
-        <f t="shared" si="7"/>
-        <v>23.136752707137308</v>
-      </c>
-      <c r="T5">
-        <f t="shared" si="8"/>
-        <v>8.5257970171630115E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="31">
-        <v>20000</v>
-      </c>
-      <c r="C6" s="32">
-        <f>(B6*4/(3*PI()))^(1/3)/100</f>
-        <v>0.20398878279639124</v>
-      </c>
-      <c r="D6" s="32">
-        <f>C6*3</f>
-        <v>0.61196634838917374</v>
-      </c>
-      <c r="E6" s="33">
-        <f>D6*9.8</f>
-        <v>5.9972702142139029</v>
-      </c>
-      <c r="F6" s="31">
-        <f>'PID &amp; Gas Output'!W8</f>
-        <v>3.6123153872598101E-6</v>
-      </c>
-      <c r="G6" s="31">
-        <f>'PID &amp; Gas Output'!T8/'Seed Train'!B8/24/3600</f>
-        <v>2.6205615232805545E-5</v>
-      </c>
-      <c r="H6" s="31">
-        <f>'PID &amp; Gas Output'!Z8</f>
-        <v>1.1611381670112299E-4</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1.2406988923882749</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>1.2111431855237487</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="2"/>
-        <v>1.0244031483789797</v>
-      </c>
-      <c r="M6" s="31">
-        <f>G6*127133</f>
-        <v>3.3315984813922674</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="4"/>
-        <v>0.86960418106101589</v>
-      </c>
-      <c r="O6">
-        <f>O7+N7-N6</f>
-        <v>2.5108064107511856</v>
-      </c>
-      <c r="P6">
-        <v>10</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="5"/>
-        <v>12.510806410751186</v>
-      </c>
-      <c r="R6">
-        <f t="shared" si="6"/>
-        <v>26.82500738643661</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="7"/>
-        <v>24.314200975685424</v>
-      </c>
-      <c r="T6">
-        <f>M6/963*SQRT(1*537/(R6^2-S6^2))</f>
-        <v>7.0750562382794037E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="31">
-        <v>80000</v>
-      </c>
-      <c r="C7" s="32">
-        <f>(B7*4/(3*PI()))^(1/3)/100</f>
-        <v>0.32381200840070401</v>
-      </c>
-      <c r="D7" s="32">
-        <f>C7*3</f>
-        <v>0.97143602520211203</v>
-      </c>
-      <c r="E7" s="33">
-        <f>D7*9.8</f>
-        <v>9.5200730469806985</v>
-      </c>
-      <c r="F7" s="31">
-        <f>'PID &amp; Gas Output'!W9</f>
-        <v>2.7738531734872098E-4</v>
-      </c>
-      <c r="G7" s="31">
-        <f>'PID &amp; Gas Output'!T9/'Seed Train'!B9/24/3600</f>
-        <v>3.1820393691348704E-4</v>
-      </c>
-      <c r="H7" s="31">
-        <f>'PID &amp; Gas Output'!Z9</f>
-        <v>4.4930211738727498E-4</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>1.2819333276136637</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>1.2111431855237487</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="2"/>
-        <v>1.058449028105048</v>
-      </c>
-      <c r="M7" s="31">
-        <f t="shared" si="3"/>
-        <v>40.454221111622346</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="4"/>
-        <v>1.3804105918122012</v>
-      </c>
-      <c r="O7">
-        <v>2</v>
-      </c>
-      <c r="P7">
-        <v>10</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="5"/>
-        <v>12</v>
-      </c>
-      <c r="R7">
-        <f t="shared" si="6"/>
-        <v>27.0804105918122</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="7"/>
-        <v>25.0804105918122</v>
-      </c>
-      <c r="T7">
-        <f t="shared" si="8"/>
-        <v>9.5309785415149742E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="31">
-        <v>400000</v>
-      </c>
-      <c r="C8" s="32">
-        <f>(B8*4/(3*PI()))^(1/3)/100</f>
-        <v>0.55371074561027633</v>
-      </c>
-      <c r="D8" s="32">
-        <f>C8*3</f>
-        <v>1.661132236830829</v>
-      </c>
-      <c r="E8" s="33">
-        <f>D8*9.8</f>
-        <v>16.279095920942126</v>
-      </c>
-      <c r="F8" s="31">
-        <f>'PID &amp; Gas Output'!W10</f>
-        <v>1.4599157214174199E-3</v>
-      </c>
-      <c r="G8" s="31">
-        <f>'PID &amp; Gas Output'!T10/'Seed Train'!B10/24/3600</f>
-        <v>1.5291703869733961E-3</v>
-      </c>
-      <c r="H8" s="31">
-        <f>'PID &amp; Gas Output'!Z10</f>
-        <v>1.829851947594E-3</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>1.3610477442057471</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>1.2111431855237487</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="2"/>
-        <v>1.1237711283634673</v>
-      </c>
-      <c r="M8" s="31">
-        <f t="shared" si="3"/>
-        <v>194.40801880708875</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="4"/>
-        <v>2.3604689085366082</v>
-      </c>
-      <c r="O8">
-        <f>O7+N7-N8</f>
-        <v>1.0199416832755932</v>
-      </c>
-      <c r="P8">
-        <v>10</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="5"/>
-        <v>11.019941683275594</v>
-      </c>
-      <c r="R8">
-        <f t="shared" si="6"/>
-        <v>27.570439750174405</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="7"/>
-        <v>26.550498066898811</v>
-      </c>
-      <c r="T8">
-        <f t="shared" si="8"/>
-        <v>0.62965796710934518</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>117</v>
-      </c>
-      <c r="R11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>123</v>
-      </c>
-      <c r="R12">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
whoops I left some stuff out:
</commit_message>
<xml_diff>
--- a/K1/FinalCodeV1/Final_OutputV3.xlsx
+++ b/K1/FinalCodeV1/Final_OutputV3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc Thomson\Documents\School Docs\College\Senior Year\Second Semester\Design\DesignCode\K1\FinalCodeV1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA50FD2-F45E-4225-884C-08F92D27B8FF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1C23D1-9548-4F1F-B3D6-D0B0ACD2E274}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" firstSheet="1" activeTab="3" xr2:uid="{246BD7EC-0C2E-4070-B711-658E9931285D}"/>
   </bookViews>
@@ -1627,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B9B371-BB26-4257-BB8E-9B4539DEEA9A}">
   <dimension ref="A1:AQ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4:AL10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1895,42 +1895,15 @@
       <c r="AB4" s="52">
         <v>43.261320828720699</v>
       </c>
-      <c r="AD4" s="26">
-        <f>('Valves and Pressure Drop'!$E2/2+100)/100*R4</f>
-        <v>2971.1899657142376</v>
-      </c>
-      <c r="AE4" s="26">
-        <f>('Valves and Pressure Drop'!$E2/2+100)/100*S4</f>
-        <v>423.55940508421031</v>
-      </c>
-      <c r="AF4" s="26">
-        <f>('Valves and Pressure Drop'!$E2/2+100)/100*T4</f>
-        <v>4499.9849891782724</v>
-      </c>
-      <c r="AG4" s="26">
-        <f>('Valves and Pressure Drop'!$E2/2+100)/100*U4</f>
-        <v>1.691525088356771E-3</v>
-      </c>
-      <c r="AH4" s="26">
-        <f>('Valves and Pressure Drop'!$E2/2+100)/100*V4</f>
-        <v>4.0437597140854914E-4</v>
-      </c>
-      <c r="AI4" s="26">
-        <f>('Valves and Pressure Drop'!$E2/2+100)/100*W4</f>
-        <v>2.7332677461372377E-3</v>
-      </c>
-      <c r="AJ4" s="26">
-        <f>('Valves and Pressure Drop'!$E2/2+100)/100*X4</f>
-        <v>5.9956369221509827E-3</v>
-      </c>
-      <c r="AK4" s="26">
-        <f>('Valves and Pressure Drop'!$E2/2+100)/100*Y4</f>
-        <v>5.5218986173857234E-4</v>
-      </c>
-      <c r="AL4" s="26">
-        <f>('Valves and Pressure Drop'!$E2/2+100)/100*Z4</f>
-        <v>6.8961826339291338E-3</v>
-      </c>
+      <c r="AD4" s="26"/>
+      <c r="AE4" s="26"/>
+      <c r="AF4" s="26"/>
+      <c r="AG4" s="26"/>
+      <c r="AH4" s="26"/>
+      <c r="AI4" s="26"/>
+      <c r="AJ4" s="26"/>
+      <c r="AK4" s="26"/>
+      <c r="AL4" s="26"/>
       <c r="AM4" s="26"/>
       <c r="AN4" s="26"/>
       <c r="AO4" s="26"/>
@@ -2022,42 +1995,15 @@
       <c r="AB5" s="52">
         <v>47.171691300973698</v>
       </c>
-      <c r="AD5" s="26">
-        <f>('Valves and Pressure Drop'!$E3/2+100)/100*R5</f>
-        <v>2633.2353924029408</v>
-      </c>
-      <c r="AE5" s="26">
-        <f>('Valves and Pressure Drop'!$E3/2+100)/100*S5</f>
-        <v>833.03462142081344</v>
-      </c>
-      <c r="AF5" s="26">
-        <f>('Valves and Pressure Drop'!$E3/2+100)/100*T5</f>
-        <v>9404.5456136775738</v>
-      </c>
-      <c r="AG5" s="26">
-        <f>('Valves and Pressure Drop'!$E3/2+100)/100*U5</f>
-        <v>5.693766698824747E-4</v>
-      </c>
-      <c r="AH5" s="26">
-        <f>('Valves and Pressure Drop'!$E3/2+100)/100*V5</f>
-        <v>2.1306415136638672E-4</v>
-      </c>
-      <c r="AI5" s="26">
-        <f>('Valves and Pressure Drop'!$E3/2+100)/100*W5</f>
-        <v>7.6409976137686679E-5</v>
-      </c>
-      <c r="AJ5" s="26">
-        <f>('Valves and Pressure Drop'!$E3/2+100)/100*X5</f>
-        <v>8.0449667402502142E-3</v>
-      </c>
-      <c r="AK5" s="26">
-        <f>('Valves and Pressure Drop'!$E3/2+100)/100*Y5</f>
-        <v>3.9715576819935472E-4</v>
-      </c>
-      <c r="AL5" s="26">
-        <f>('Valves and Pressure Drop'!$E3/2+100)/100*Z5</f>
-        <v>4.0420732797868111E-3</v>
-      </c>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="26"/>
+      <c r="AG5" s="26"/>
+      <c r="AH5" s="26"/>
+      <c r="AI5" s="26"/>
+      <c r="AJ5" s="26"/>
+      <c r="AK5" s="26"/>
+      <c r="AL5" s="26"/>
     </row>
     <row r="6" spans="1:43" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
@@ -2144,42 +2090,15 @@
       <c r="AB6" s="52">
         <v>59.6570893210219</v>
       </c>
-      <c r="AD6" s="26">
-        <f>('Valves and Pressure Drop'!$E4/2+100)/100*R6</f>
-        <v>234.64166774833521</v>
-      </c>
-      <c r="AE6" s="26">
-        <f>('Valves and Pressure Drop'!$E4/2+100)/100*S6</f>
-        <v>18.791112034980188</v>
-      </c>
-      <c r="AF6" s="26">
-        <f>('Valves and Pressure Drop'!$E4/2+100)/100*T6</f>
-        <v>71.835939889063837</v>
-      </c>
-      <c r="AG6" s="26">
-        <f>('Valves and Pressure Drop'!$E4/2+100)/100*U6</f>
-        <v>4.4476926974113164E-4</v>
-      </c>
-      <c r="AH6" s="26">
-        <f>('Valves and Pressure Drop'!$E4/2+100)/100*V6</f>
-        <v>7.8087064424940493E-5</v>
-      </c>
-      <c r="AI6" s="26">
-        <f>('Valves and Pressure Drop'!$E4/2+100)/100*W6</f>
-        <v>1.4156439450011557E-4</v>
-      </c>
-      <c r="AJ6" s="26">
-        <f>('Valves and Pressure Drop'!$E4/2+100)/100*X6</f>
-        <v>1.3169543596330505E-3</v>
-      </c>
-      <c r="AK6" s="26">
-        <f>('Valves and Pressure Drop'!$E4/2+100)/100*Y6</f>
-        <v>1.1467666473032697E-4</v>
-      </c>
-      <c r="AL6" s="26">
-        <f>('Valves and Pressure Drop'!$E4/2+100)/100*Z6</f>
-        <v>9.7755243010692818E-4</v>
-      </c>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
+      <c r="AG6" s="26"/>
+      <c r="AH6" s="26"/>
+      <c r="AI6" s="26"/>
+      <c r="AJ6" s="26"/>
+      <c r="AK6" s="26"/>
+      <c r="AL6" s="26"/>
     </row>
     <row r="7" spans="1:43" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
@@ -2266,42 +2185,15 @@
       <c r="AB7" s="52">
         <v>55.367097463428401</v>
       </c>
-      <c r="AD7" s="26">
-        <f>('Valves and Pressure Drop'!$E5/2+100)/100*R7</f>
-        <v>221.13073239351695</v>
-      </c>
-      <c r="AE7" s="26">
-        <f>('Valves and Pressure Drop'!$E5/2+100)/100*S7</f>
-        <v>20.174934938929258</v>
-      </c>
-      <c r="AF7" s="26">
-        <f>('Valves and Pressure Drop'!$E5/2+100)/100*T7</f>
-        <v>100.10447519388711</v>
-      </c>
-      <c r="AG7" s="26">
-        <f>('Valves and Pressure Drop'!$E5/2+100)/100*U7</f>
-        <v>4.6463569228962555E-4</v>
-      </c>
-      <c r="AH7" s="26">
-        <f>('Valves and Pressure Drop'!$E5/2+100)/100*V7</f>
-        <v>8.59485696280264E-5</v>
-      </c>
-      <c r="AI7" s="26">
-        <f>('Valves and Pressure Drop'!$E5/2+100)/100*W7</f>
-        <v>2.9590743353996677E-4</v>
-      </c>
-      <c r="AJ7" s="26">
-        <f>('Valves and Pressure Drop'!$E5/2+100)/100*X7</f>
-        <v>1.23466929288472E-3</v>
-      </c>
-      <c r="AK7" s="26">
-        <f>('Valves and Pressure Drop'!$E5/2+100)/100*Y7</f>
-        <v>1.1266731486079619E-4</v>
-      </c>
-      <c r="AL7" s="26">
-        <f>('Valves and Pressure Drop'!$E5/2+100)/100*Z7</f>
-        <v>1.0393115740568134E-3</v>
-      </c>
+      <c r="AD7" s="26"/>
+      <c r="AE7" s="26"/>
+      <c r="AF7" s="26"/>
+      <c r="AG7" s="26"/>
+      <c r="AH7" s="26"/>
+      <c r="AI7" s="26"/>
+      <c r="AJ7" s="26"/>
+      <c r="AK7" s="26"/>
+      <c r="AL7" s="26"/>
     </row>
     <row r="8" spans="1:43" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
@@ -2388,42 +2280,15 @@
       <c r="AB8" s="52">
         <v>41.630397373854798</v>
       </c>
-      <c r="AD8" s="26">
-        <f>('Valves and Pressure Drop'!$E6/2+100)/100*R8</f>
-        <v>60.040529956153776</v>
-      </c>
-      <c r="AE8" s="26">
-        <f>('Valves and Pressure Drop'!$E6/2+100)/100*S8</f>
-        <v>7.8622683545621497</v>
-      </c>
-      <c r="AF8" s="26">
-        <f>('Valves and Pressure Drop'!$E6/2+100)/100*T8</f>
-        <v>5.8968833717914384</v>
-      </c>
-      <c r="AG8" s="26">
-        <f>('Valves and Pressure Drop'!$E6/2+100)/100*U8</f>
-        <v>1.8226446525309369E-4</v>
-      </c>
-      <c r="AH8" s="26">
-        <f>('Valves and Pressure Drop'!$E6/2+100)/100*V8</f>
-        <v>3.5321311842915764E-5</v>
-      </c>
-      <c r="AI8" s="26">
-        <f>('Valves and Pressure Drop'!$E6/2+100)/100*W8</f>
-        <v>3.8322038282907316E-6</v>
-      </c>
-      <c r="AJ8" s="26">
-        <f>('Valves and Pressure Drop'!$E6/2+100)/100*X8</f>
-        <v>3.4294624062456797E-4</v>
-      </c>
-      <c r="AK8" s="26">
-        <f>('Valves and Pressure Drop'!$E6/2+100)/100*Y8</f>
-        <v>4.148301618471198E-5</v>
-      </c>
-      <c r="AL8" s="26">
-        <f>('Valves and Pressure Drop'!$E6/2+100)/100*Z8</f>
-        <v>1.2318188341163466E-4</v>
-      </c>
+      <c r="AD8" s="26"/>
+      <c r="AE8" s="26"/>
+      <c r="AF8" s="26"/>
+      <c r="AG8" s="26"/>
+      <c r="AH8" s="26"/>
+      <c r="AI8" s="26"/>
+      <c r="AJ8" s="26"/>
+      <c r="AK8" s="26"/>
+      <c r="AL8" s="26"/>
     </row>
     <row r="9" spans="1:43" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
@@ -2510,42 +2375,15 @@
       <c r="AB9" s="52">
         <v>43.3637076844864</v>
       </c>
-      <c r="AD9" s="26">
-        <f>('Valves and Pressure Drop'!$E7/2+100)/100*R9</f>
-        <v>89.014237658392489</v>
-      </c>
-      <c r="AE9" s="26">
-        <f>('Valves and Pressure Drop'!$E7/2+100)/100*S9</f>
-        <v>12.142424036277747</v>
-      </c>
-      <c r="AF9" s="26">
-        <f>('Valves and Pressure Drop'!$E7/2+100)/100*T9</f>
-        <v>63.965593572473615</v>
-      </c>
-      <c r="AG9" s="26">
-        <f>('Valves and Pressure Drop'!$E7/2+100)/100*U9</f>
-        <v>3.3874133140888399E-4</v>
-      </c>
-      <c r="AH9" s="26">
-        <f>('Valves and Pressure Drop'!$E7/2+100)/100*V9</f>
-        <v>6.4002610316090771E-5</v>
-      </c>
-      <c r="AI9" s="26">
-        <f>('Valves and Pressure Drop'!$E7/2+100)/100*W9</f>
-        <v>3.0442110038337965E-4</v>
-      </c>
-      <c r="AJ9" s="26">
-        <f>('Valves and Pressure Drop'!$E7/2+100)/100*X9</f>
-        <v>5.3520170009430806E-4</v>
-      </c>
-      <c r="AK9" s="26">
-        <f>('Valves and Pressure Drop'!$E7/2+100)/100*Y9</f>
-        <v>7.1970394722008338E-5</v>
-      </c>
-      <c r="AL9" s="26">
-        <f>('Valves and Pressure Drop'!$E7/2+100)/100*Z9</f>
-        <v>4.9309403355212356E-4</v>
-      </c>
+      <c r="AD9" s="26"/>
+      <c r="AE9" s="26"/>
+      <c r="AF9" s="26"/>
+      <c r="AG9" s="26"/>
+      <c r="AH9" s="26"/>
+      <c r="AI9" s="26"/>
+      <c r="AJ9" s="26"/>
+      <c r="AK9" s="26"/>
+      <c r="AL9" s="26"/>
     </row>
     <row r="10" spans="1:43" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
@@ -2632,42 +2470,15 @@
       <c r="AB10" s="53">
         <v>39.515087305645999</v>
       </c>
-      <c r="AD10" s="26">
-        <f>('Valves and Pressure Drop'!$E8/2+100)/100*R10</f>
-        <v>178.84789517335156</v>
-      </c>
-      <c r="AE10" s="26">
-        <f>('Valves and Pressure Drop'!$E8/2+100)/100*S10</f>
-        <v>37.925884578749915</v>
-      </c>
-      <c r="AF10" s="26">
-        <f>('Valves and Pressure Drop'!$E8/2+100)/100*T10</f>
-        <v>379.3064411825676</v>
-      </c>
-      <c r="AG10" s="26">
-        <f>('Valves and Pressure Drop'!$E8/2+100)/100*U10</f>
-        <v>4.9307296644687261E-4</v>
-      </c>
-      <c r="AH10" s="26">
-        <f>('Valves and Pressure Drop'!$E8/2+100)/100*V10</f>
-        <v>1.7470773019929756E-4</v>
-      </c>
-      <c r="AI10" s="26">
-        <f>('Valves and Pressure Drop'!$E8/2+100)/100*W10</f>
-        <v>1.7072490708934893E-3</v>
-      </c>
-      <c r="AJ10" s="26">
-        <f>('Valves and Pressure Drop'!$E8/2+100)/100*X10</f>
-        <v>9.339928442901864E-4</v>
-      </c>
-      <c r="AK10" s="26">
-        <f>('Valves and Pressure Drop'!$E8/2+100)/100*Y10</f>
-        <v>1.8683870978723559E-4</v>
-      </c>
-      <c r="AL10" s="26">
-        <f>('Valves and Pressure Drop'!$E8/2+100)/100*Z10</f>
-        <v>2.1398584805768267E-3</v>
-      </c>
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="26"/>
+      <c r="AF10" s="26"/>
+      <c r="AG10" s="26"/>
+      <c r="AH10" s="26"/>
+      <c r="AI10" s="26"/>
+      <c r="AJ10" s="26"/>
+      <c r="AK10" s="26"/>
+      <c r="AL10" s="26"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="X12" s="31"/>
@@ -3278,8 +3089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AC2659-451F-4A9A-A90E-79F819C9DD82}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3453,8 +3264,7 @@
         <v>23.986345056475798</v>
       </c>
       <c r="S2" s="32">
-        <f>R2-O2</f>
-        <v>18.986345056475798</v>
+        <v>0</v>
       </c>
       <c r="T2" s="59">
         <f>R2-14.7</f>
@@ -3463,19 +3273,19 @@
       <c r="U2" s="32"/>
       <c r="V2" s="32">
         <f>M2/963*SQRT(1*537/(R2^2-S2^2))</f>
-        <v>0.95420393896487787</v>
+        <v>0.58312062273158605</v>
       </c>
       <c r="W2" s="32">
         <f>F2/963*SQRT(1*537/(R2^2-S2^2))*127133*0.95</f>
-        <v>0.47571808743980704</v>
+        <v>0.29071461148389777</v>
       </c>
       <c r="X2" s="32">
         <f>H2/963*SQRT(1*537/(R2^2-S2^2))*127133*1.05</f>
-        <v>1.3266059352463029</v>
+        <v>0.81069805676909468</v>
       </c>
       <c r="Y2" s="32">
         <f>X2/W2</f>
-        <v>2.7886388394138142</v>
+        <v>2.7886388394138146</v>
       </c>
       <c r="Z2" t="s">
         <v>123</v>

</xml_diff>